<commit_message>
cleanup data for Q07.4
</commit_message>
<xml_diff>
--- a/Analysis/All Results by Region.xlsx
+++ b/Analysis/All Results by Region.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\un50sc-foc-fpos\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F411A035-5589-4F4E-AF34-E09B04628F80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624C5433-918B-4B98-88EC-074068AEFB6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{96E8121E-4952-4330-BB1B-72D20337AD4A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8228" uniqueCount="1669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8713" uniqueCount="1766">
   <si>
     <t>QuestionID</t>
   </si>
@@ -5037,6 +5037,297 @@
   </si>
   <si>
     <t>there are some contradiction between other laws and the STAT law</t>
+  </si>
+  <si>
+    <t>Q07.1</t>
+  </si>
+  <si>
+    <t>Existence of a general statistics law in the country</t>
+  </si>
+  <si>
+    <t>Q07.2</t>
+  </si>
+  <si>
+    <t>Aspects of the NSS covered by regulations (e.g. Statistical Law, presidential decrees)</t>
+  </si>
+  <si>
+    <t>The definition of official statistics</t>
+  </si>
+  <si>
+    <t>The body responsible for statistics and its responsibilities</t>
+  </si>
+  <si>
+    <t>The status, mandate and functions of the NSO</t>
+  </si>
+  <si>
+    <t>The role and status of the chief statistician</t>
+  </si>
+  <si>
+    <t>The staff of the NSO</t>
+  </si>
+  <si>
+    <t>The role and membership of the national statistical council</t>
+  </si>
+  <si>
+    <t>The coordination of statistical activities across government</t>
+  </si>
+  <si>
+    <t>The role and the responsibilities of agencies other than the NSO</t>
+  </si>
+  <si>
+    <t>The matters to be covered in the statistical work program</t>
+  </si>
+  <si>
+    <t>Sanctions for not responding to mandatory statistical enquiries</t>
+  </si>
+  <si>
+    <t>Access to administrative data</t>
+  </si>
+  <si>
+    <t>Presumption of publication and the acceptable conditions for not publishing data collected</t>
+  </si>
+  <si>
+    <t>Secrecy, confidentiality and privacy obligations (including sanctions for non-compliance)</t>
+  </si>
+  <si>
+    <t>Participation in international statistical activities</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>Access to administrative data is not specifically mentioned by any law but it is mentioned that the Statistician-General can collect any data. Presumption on publication: there is a general provision that the Statistician-General can discontinue any data collection process.</t>
+  </si>
+  <si>
+    <t>Creation of sectoral statistical committees, and cross-posting of PSA staff in other agencies to provide technical assistance</t>
+  </si>
+  <si>
+    <t>Designation of NSO as coordinator of NSS; Conditions under which microdata access may be granted</t>
+  </si>
+  <si>
+    <t>Role of Minister responsible; Oath of office (secrecy); Provisions for sharing and disclosure</t>
+  </si>
+  <si>
+    <t>Statistical classifications to be applied by NSO and other concerned authorities; Quality management system in the NBS and other producers of official statistics</t>
+  </si>
+  <si>
+    <t>Q07.2a</t>
+  </si>
+  <si>
+    <t>Agencies other than NSO whose role and responsibilities are covered by the law</t>
+  </si>
+  <si>
+    <t>Statistical offices at the sub-national level (region, province, etc.)</t>
+  </si>
+  <si>
+    <t>Statistical services in line ministries</t>
+  </si>
+  <si>
+    <t>Statistical services in the Central Bank</t>
+  </si>
+  <si>
+    <t>Custodians of administrative data</t>
+  </si>
+  <si>
+    <t>Chambers of commerce or other business networks</t>
+  </si>
+  <si>
+    <t>Trade unions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistical research and training centres </t>
+  </si>
+  <si>
+    <t>Private institutions</t>
+  </si>
+  <si>
+    <t>Supra-national bodies (e.g. Eurostat)</t>
+  </si>
+  <si>
+    <t>Australian Institute for Health and Welfare (AIHW) which is a statutory body</t>
+  </si>
+  <si>
+    <t>Other ELSS agencies (National Documentation Centre, Hellenic Telecommunications and Post Commission)</t>
+  </si>
+  <si>
+    <t>Please, see: https://statistiques.public.lu/en/actors/statec/legalbasis/LawSTATEC.pdf. Statec's law covers the missions of the Committee on Public Statistics which is made up of representatives of administrations, ministries and observatories active in holding, producing and disseminating statistics.</t>
+  </si>
+  <si>
+    <t>State institutions, which provide official statistics</t>
+  </si>
+  <si>
+    <t>Statistical services under line ministries which are gazetted under the Statistics Act</t>
+  </si>
+  <si>
+    <t>The informants</t>
+  </si>
+  <si>
+    <t>Q07.2b</t>
+  </si>
+  <si>
+    <t>How the enforceability "sanctions for not responding to mandatory statistical enquiries” is decided for specific surveys</t>
+  </si>
+  <si>
+    <t>According to the type of survey</t>
+  </si>
+  <si>
+    <t>According to whether it belongs to the core set of statistical enquiries</t>
+  </si>
+  <si>
+    <t>Ad-hoc</t>
+  </si>
+  <si>
+    <t>All surveys are mandatory</t>
+  </si>
+  <si>
+    <t>By persuasion, re-contacts.</t>
+  </si>
+  <si>
+    <t>If the data quality of a voluntary survey is probably insufficient, it will be classified as mandatory for being abke to collect high quality data</t>
+  </si>
+  <si>
+    <t>Sanctions apply only for surveys that are mandatory. Specific criteria for mandatory surveys is set out in policy, and include factors such as where the survey results meet specific requirements of other federal and provincial statutes and regulations, or the results may affect domestic and international financial and commodity markets.</t>
+  </si>
+  <si>
+    <t>The households, individuals and in some cases farms are not obliged to participate in the statistical surveys. All business surveys are mandatory.</t>
+  </si>
+  <si>
+    <t>The surveys conducted under Statistics Act</t>
+  </si>
+  <si>
+    <t>When conducting the surveys, according to the programme of statistical work, the respondents shall be obliged: a) to provide producers of official statistics, free of charge, with reliable and complete data in the manner established by the producer of official statistics concerned; b) to ensure free access for the representatives of producers of official statistics to the supporting documents and, where necessary, to the office and production premises and to the land, according to the legal provisions</t>
+  </si>
+  <si>
+    <t>the list of surveys with mandatory response as well as the list of surveys where non-response is sanctioned are approved, according to the national statistical law, with a Decree by the President of the Italian Republic which is the same decree that approves the National Statistical Programme</t>
+  </si>
+  <si>
+    <t>Q07.3</t>
+  </si>
+  <si>
+    <t>How the NSO has encouraged respondents to answer surveys during the past five years</t>
+  </si>
+  <si>
+    <t>By launching awareness campaigns prior to censuses or large surveys</t>
+  </si>
+  <si>
+    <t>By sending pre-announcement letters</t>
+  </si>
+  <si>
+    <t>By requesting informed consent</t>
+  </si>
+  <si>
+    <t>By providing an explanatory text on the front page of the survey</t>
+  </si>
+  <si>
+    <t>By applying fines for not responding</t>
+  </si>
+  <si>
+    <t>By declaring the census day national holiday</t>
+  </si>
+  <si>
+    <t>By following up with non-responders</t>
+  </si>
+  <si>
+    <t>By sending statistics back to the respondens where they can see where they are positioned in relation to the statistical result is done in a few cases</t>
+  </si>
+  <si>
+    <t>HBS uses a reward practice for respondents providing detailed answers according the agenda.</t>
+  </si>
+  <si>
+    <t>In some statistical surveys targeted at households incentives are given to the respondents</t>
+  </si>
+  <si>
+    <t>Incentives (promotional items) to respondents</t>
+  </si>
+  <si>
+    <t>Incentives for participation (entry into national raffles); training survey staff in how to encourage participation by reluctant respondents</t>
+  </si>
+  <si>
+    <t>Mandatory to respond for surveys conducted under the Statistics Act</t>
+  </si>
+  <si>
+    <t>National Statistics Day on 20 October</t>
+  </si>
+  <si>
+    <t>The Census Bureau makes plant visits to talk to non-respondants for certain surveys, like M3.</t>
+  </si>
+  <si>
+    <t>The respondent's calendar is posted on Belstat's official website, as well as a schedule of primary data collection in electronic form that contains information on the start date and the deadline for statistical reports collection for each statistical survey for each reporting period; The online report collection provides the possibility for respondent to view an individual list of required reporting forms.</t>
+  </si>
+  <si>
+    <t>sending paper reminders, telephone reminders, visiting companies</t>
+  </si>
+  <si>
+    <t>social media and announcement in public places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q07.4 </t>
+  </si>
+  <si>
+    <t>Person/office within the government to whom the head of the NSO reports</t>
+  </si>
+  <si>
+    <t>Australian Treasury</t>
+  </si>
+  <si>
+    <t>Cabinet or Council of Ministers</t>
+  </si>
+  <si>
+    <t>Consejo Directivo del INEC</t>
+  </si>
+  <si>
+    <t>Generally to the Prime Minister (first answer) and to the Statistical Council as regards the annual program of statistical surveys of official statistics</t>
+  </si>
+  <si>
+    <t>Head of the State Services</t>
+  </si>
+  <si>
+    <t>Heads of US statistical agencies usually report to their Department.</t>
+  </si>
+  <si>
+    <t>Minister of Prime Minister's Office</t>
+  </si>
+  <si>
+    <t>Ministry of Economic Development</t>
+  </si>
+  <si>
+    <t>Ministry of Finance and Economic Development</t>
+  </si>
+  <si>
+    <t>Ministry of Treasury and Finance</t>
+  </si>
+  <si>
+    <t>Ministry of economic affairs, industry or trade</t>
+  </si>
+  <si>
+    <t>Ministry of finance or comptroller general</t>
+  </si>
+  <si>
+    <t>Ministry of planning or development</t>
+  </si>
+  <si>
+    <t>Ministry of the interior</t>
+  </si>
+  <si>
+    <t>Parliament/Congress</t>
+  </si>
+  <si>
+    <t>Planning or development authority</t>
+  </si>
+  <si>
+    <t>Prime Minister, chancellor or President</t>
+  </si>
+  <si>
+    <t>To general public</t>
+  </si>
+  <si>
+    <t>the Presidency of the Council of Ministers (artt.14 and 24 of statistical law)</t>
+  </si>
+  <si>
+    <t>the head of the NSO reports to the Ministry of economy and finances</t>
   </si>
 </sst>
 </file>
@@ -6109,10 +6400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCEED60D-61AB-4CB8-AD9A-C5E4119AA60E}">
-  <dimension ref="A1:W1780"/>
+  <dimension ref="A1:W1882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1755" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1764" sqref="B1764"/>
+    <sheetView tabSelected="1" topLeftCell="A1855" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1863" sqref="L1863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12530,7 +12821,7 @@
       </c>
       <c r="V168" s="66"/>
       <c r="W168" s="67">
-        <f>Q168+W169</f>
+        <f t="shared" ref="W168:W174" si="5">Q168+W169</f>
         <v>56.989247311827903</v>
       </c>
     </row>
@@ -12600,7 +12891,7 @@
       </c>
       <c r="V169" s="66"/>
       <c r="W169" s="67">
-        <f>Q169+W170</f>
+        <f t="shared" si="5"/>
         <v>52.688172043010702</v>
       </c>
     </row>
@@ -12670,7 +12961,7 @@
       </c>
       <c r="V170" s="66"/>
       <c r="W170" s="67">
-        <f>Q170+W171</f>
+        <f t="shared" si="5"/>
         <v>30.107526881720403</v>
       </c>
     </row>
@@ -12740,7 +13031,7 @@
       </c>
       <c r="V171" s="66"/>
       <c r="W171" s="67">
-        <f>Q171+W172</f>
+        <f t="shared" si="5"/>
         <v>23.655913978494596</v>
       </c>
     </row>
@@ -12802,7 +13093,7 @@
       </c>
       <c r="V172" s="66"/>
       <c r="W172" s="67">
-        <f>Q172+W173</f>
+        <f t="shared" si="5"/>
         <v>7.5268817204300991</v>
       </c>
     </row>
@@ -12864,7 +13155,7 @@
       </c>
       <c r="V173" s="66"/>
       <c r="W173" s="67">
-        <f>Q173+W174</f>
+        <f t="shared" si="5"/>
         <v>4.3010752688171996</v>
       </c>
     </row>
@@ -12922,7 +13213,7 @@
       </c>
       <c r="V174" s="66"/>
       <c r="W174" s="67">
-        <f>Q174+W175</f>
+        <f t="shared" si="5"/>
         <v>2.1505376344085998</v>
       </c>
     </row>
@@ -12963,19 +13254,19 @@
         <v>1.0752688172042999</v>
       </c>
       <c r="R175" s="68">
-        <f t="shared" ref="R175:U175" si="5">L175</f>
+        <f t="shared" ref="R175:U175" si="6">L175</f>
         <v>0</v>
       </c>
       <c r="S175" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.6923076923076898</v>
       </c>
       <c r="T175" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U175" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V175" s="68"/>
@@ -67285,9 +67576,3804 @@
       <c r="P1780" s="78"/>
       <c r="Q1780" s="111"/>
     </row>
+    <row r="1781" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1782" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1782" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1782" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1782" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1782" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1782" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1782" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1782" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1782" s="97" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1782" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1782" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1782" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1782" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1782" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1782" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1782" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1782" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1782" s="99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1783" s="3" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B1783" s="4" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C1783" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1783" s="4"/>
+      <c r="E1783" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1783" s="5"/>
+      <c r="G1783" s="5">
+        <v>1</v>
+      </c>
+      <c r="H1783" s="5">
+        <v>2</v>
+      </c>
+      <c r="I1783" s="5"/>
+      <c r="J1783" s="5"/>
+      <c r="K1783" s="18">
+        <v>3</v>
+      </c>
+      <c r="L1783" s="64"/>
+      <c r="M1783" s="64">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1783" s="64">
+        <v>8.3333333333333304</v>
+      </c>
+      <c r="O1783" s="64"/>
+      <c r="P1783" s="64"/>
+      <c r="Q1783" s="65">
+        <v>3.2258064516128999</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1784" s="9" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B1784" s="10" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C1784" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1784" s="10"/>
+      <c r="E1784" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1784" s="11">
+        <v>17</v>
+      </c>
+      <c r="G1784" s="11">
+        <v>12</v>
+      </c>
+      <c r="H1784" s="11">
+        <v>22</v>
+      </c>
+      <c r="I1784" s="11">
+        <v>35</v>
+      </c>
+      <c r="J1784" s="11">
+        <v>4</v>
+      </c>
+      <c r="K1784" s="20">
+        <v>90</v>
+      </c>
+      <c r="L1784" s="68">
+        <v>100</v>
+      </c>
+      <c r="M1784" s="68">
+        <v>92.307692307692307</v>
+      </c>
+      <c r="N1784" s="68">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="O1784" s="68">
+        <v>100</v>
+      </c>
+      <c r="P1784" s="68">
+        <v>100</v>
+      </c>
+      <c r="Q1784" s="69">
+        <v>96.774193548387103</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1786" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1786" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1786" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1786" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1786" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1786" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1786" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1786" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1786" s="97" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1786" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1786" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1786" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1786" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1786" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1786" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1786" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1786" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1786" s="99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1787" s="50" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1787" s="51" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1787" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1787" s="51" t="s">
+        <v>1674</v>
+      </c>
+      <c r="E1787" s="51"/>
+      <c r="F1787" s="52">
+        <v>17</v>
+      </c>
+      <c r="G1787" s="52">
+        <v>12</v>
+      </c>
+      <c r="H1787" s="52">
+        <v>22</v>
+      </c>
+      <c r="I1787" s="52">
+        <v>33</v>
+      </c>
+      <c r="J1787" s="52">
+        <v>4</v>
+      </c>
+      <c r="K1787" s="53">
+        <v>88</v>
+      </c>
+      <c r="L1787" s="86">
+        <v>100</v>
+      </c>
+      <c r="M1787" s="86">
+        <v>92.307692307692307</v>
+      </c>
+      <c r="N1787" s="86">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="O1787" s="86">
+        <v>94.285714285714306</v>
+      </c>
+      <c r="P1787" s="86">
+        <v>100</v>
+      </c>
+      <c r="Q1787" s="87">
+        <v>94.623655913978496</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1788" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1788" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1788" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1788" s="55" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E1788" s="55"/>
+      <c r="F1788" s="56">
+        <v>15</v>
+      </c>
+      <c r="G1788" s="56">
+        <v>13</v>
+      </c>
+      <c r="H1788" s="56">
+        <v>20</v>
+      </c>
+      <c r="I1788" s="56">
+        <v>33</v>
+      </c>
+      <c r="J1788" s="56">
+        <v>4</v>
+      </c>
+      <c r="K1788" s="57">
+        <v>85</v>
+      </c>
+      <c r="L1788" s="88">
+        <v>88.235294117647101</v>
+      </c>
+      <c r="M1788" s="88">
+        <v>100</v>
+      </c>
+      <c r="N1788" s="88">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="O1788" s="88">
+        <v>94.285714285714306</v>
+      </c>
+      <c r="P1788" s="88">
+        <v>100</v>
+      </c>
+      <c r="Q1788" s="89">
+        <v>91.397849462365599</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1789" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1789" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1789" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1789" s="55" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E1789" s="55"/>
+      <c r="F1789" s="56">
+        <v>16</v>
+      </c>
+      <c r="G1789" s="56">
+        <v>13</v>
+      </c>
+      <c r="H1789" s="56">
+        <v>19</v>
+      </c>
+      <c r="I1789" s="56">
+        <v>32</v>
+      </c>
+      <c r="J1789" s="56">
+        <v>4</v>
+      </c>
+      <c r="K1789" s="57">
+        <v>84</v>
+      </c>
+      <c r="L1789" s="88">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="M1789" s="88">
+        <v>100</v>
+      </c>
+      <c r="N1789" s="88">
+        <v>79.1666666666667</v>
+      </c>
+      <c r="O1789" s="88">
+        <v>91.428571428571402</v>
+      </c>
+      <c r="P1789" s="88">
+        <v>100</v>
+      </c>
+      <c r="Q1789" s="89">
+        <v>90.322580645161295</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1790" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1790" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1790" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1790" s="55" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E1790" s="55"/>
+      <c r="F1790" s="56">
+        <v>17</v>
+      </c>
+      <c r="G1790" s="56">
+        <v>12</v>
+      </c>
+      <c r="H1790" s="56">
+        <v>15</v>
+      </c>
+      <c r="I1790" s="56">
+        <v>33</v>
+      </c>
+      <c r="J1790" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1790" s="57">
+        <v>80</v>
+      </c>
+      <c r="L1790" s="88">
+        <v>100</v>
+      </c>
+      <c r="M1790" s="88">
+        <v>92.307692307692307</v>
+      </c>
+      <c r="N1790" s="88">
+        <v>62.5</v>
+      </c>
+      <c r="O1790" s="88">
+        <v>94.285714285714306</v>
+      </c>
+      <c r="P1790" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1790" s="89">
+        <v>86.021505376344095</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1791" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1791" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1791" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1791" s="55" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E1791" s="55"/>
+      <c r="F1791" s="56">
+        <v>17</v>
+      </c>
+      <c r="G1791" s="56">
+        <v>11</v>
+      </c>
+      <c r="H1791" s="56">
+        <v>18</v>
+      </c>
+      <c r="I1791" s="56">
+        <v>28</v>
+      </c>
+      <c r="J1791" s="56">
+        <v>4</v>
+      </c>
+      <c r="K1791" s="57">
+        <v>78</v>
+      </c>
+      <c r="L1791" s="88">
+        <v>100</v>
+      </c>
+      <c r="M1791" s="88">
+        <v>84.615384615384599</v>
+      </c>
+      <c r="N1791" s="88">
+        <v>75</v>
+      </c>
+      <c r="O1791" s="88">
+        <v>80</v>
+      </c>
+      <c r="P1791" s="88">
+        <v>100</v>
+      </c>
+      <c r="Q1791" s="89">
+        <v>83.870967741935502</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1792" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1792" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1792" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1792" s="55" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E1792" s="55"/>
+      <c r="F1792" s="56">
+        <v>15</v>
+      </c>
+      <c r="G1792" s="56">
+        <v>10</v>
+      </c>
+      <c r="H1792" s="56">
+        <v>18</v>
+      </c>
+      <c r="I1792" s="56">
+        <v>30</v>
+      </c>
+      <c r="J1792" s="56">
+        <v>4</v>
+      </c>
+      <c r="K1792" s="57">
+        <v>77</v>
+      </c>
+      <c r="L1792" s="88">
+        <v>88.235294117647101</v>
+      </c>
+      <c r="M1792" s="88">
+        <v>76.923076923076906</v>
+      </c>
+      <c r="N1792" s="88">
+        <v>75</v>
+      </c>
+      <c r="O1792" s="88">
+        <v>85.714285714285694</v>
+      </c>
+      <c r="P1792" s="88">
+        <v>100</v>
+      </c>
+      <c r="Q1792" s="89">
+        <v>82.795698924731198</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1793" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1793" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1793" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1793" s="55" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E1793" s="55"/>
+      <c r="F1793" s="56">
+        <v>16</v>
+      </c>
+      <c r="G1793" s="56">
+        <v>10</v>
+      </c>
+      <c r="H1793" s="56">
+        <v>18</v>
+      </c>
+      <c r="I1793" s="56">
+        <v>29</v>
+      </c>
+      <c r="J1793" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1793" s="57">
+        <v>76</v>
+      </c>
+      <c r="L1793" s="88">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="M1793" s="88">
+        <v>76.923076923076906</v>
+      </c>
+      <c r="N1793" s="88">
+        <v>75</v>
+      </c>
+      <c r="O1793" s="88">
+        <v>82.857142857142904</v>
+      </c>
+      <c r="P1793" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1793" s="89">
+        <v>81.720430107526894</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1794" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1794" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1794" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1794" s="55" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E1794" s="55"/>
+      <c r="F1794" s="56">
+        <v>14</v>
+      </c>
+      <c r="G1794" s="56">
+        <v>9</v>
+      </c>
+      <c r="H1794" s="56">
+        <v>15</v>
+      </c>
+      <c r="I1794" s="56">
+        <v>33</v>
+      </c>
+      <c r="J1794" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1794" s="57">
+        <v>74</v>
+      </c>
+      <c r="L1794" s="88">
+        <v>82.352941176470594</v>
+      </c>
+      <c r="M1794" s="88">
+        <v>69.230769230769198</v>
+      </c>
+      <c r="N1794" s="88">
+        <v>62.5</v>
+      </c>
+      <c r="O1794" s="88">
+        <v>94.285714285714306</v>
+      </c>
+      <c r="P1794" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1794" s="89">
+        <v>79.569892473118301</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1795" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1795" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1795" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1795" s="55" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E1795" s="55"/>
+      <c r="F1795" s="56">
+        <v>17</v>
+      </c>
+      <c r="G1795" s="56">
+        <v>9</v>
+      </c>
+      <c r="H1795" s="56">
+        <v>13</v>
+      </c>
+      <c r="I1795" s="56">
+        <v>26</v>
+      </c>
+      <c r="J1795" s="56">
+        <v>2</v>
+      </c>
+      <c r="K1795" s="57">
+        <v>67</v>
+      </c>
+      <c r="L1795" s="88">
+        <v>100</v>
+      </c>
+      <c r="M1795" s="88">
+        <v>69.230769230769198</v>
+      </c>
+      <c r="N1795" s="88">
+        <v>54.1666666666667</v>
+      </c>
+      <c r="O1795" s="88">
+        <v>74.285714285714306</v>
+      </c>
+      <c r="P1795" s="88">
+        <v>50</v>
+      </c>
+      <c r="Q1795" s="89">
+        <v>72.043010752688204</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1796" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1796" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1796" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1796" s="55" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E1796" s="55"/>
+      <c r="F1796" s="56">
+        <v>13</v>
+      </c>
+      <c r="G1796" s="56">
+        <v>6</v>
+      </c>
+      <c r="H1796" s="56">
+        <v>18</v>
+      </c>
+      <c r="I1796" s="56">
+        <v>25</v>
+      </c>
+      <c r="J1796" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1796" s="57">
+        <v>65</v>
+      </c>
+      <c r="L1796" s="88">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="M1796" s="88">
+        <v>46.153846153846203</v>
+      </c>
+      <c r="N1796" s="88">
+        <v>75</v>
+      </c>
+      <c r="O1796" s="88">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="P1796" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1796" s="89">
+        <v>69.892473118279597</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1797" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1797" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1797" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1797" s="55" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E1797" s="55"/>
+      <c r="F1797" s="56">
+        <v>14</v>
+      </c>
+      <c r="G1797" s="56">
+        <v>9</v>
+      </c>
+      <c r="H1797" s="56">
+        <v>15</v>
+      </c>
+      <c r="I1797" s="56">
+        <v>23</v>
+      </c>
+      <c r="J1797" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1797" s="57">
+        <v>64</v>
+      </c>
+      <c r="L1797" s="88">
+        <v>82.352941176470594</v>
+      </c>
+      <c r="M1797" s="88">
+        <v>69.230769230769198</v>
+      </c>
+      <c r="N1797" s="88">
+        <v>62.5</v>
+      </c>
+      <c r="O1797" s="88">
+        <v>65.714285714285694</v>
+      </c>
+      <c r="P1797" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1797" s="89">
+        <v>68.817204301075293</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1798" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1798" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1798" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1798" s="55" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E1798" s="55"/>
+      <c r="F1798" s="56">
+        <v>9</v>
+      </c>
+      <c r="G1798" s="56">
+        <v>9</v>
+      </c>
+      <c r="H1798" s="56">
+        <v>14</v>
+      </c>
+      <c r="I1798" s="56">
+        <v>27</v>
+      </c>
+      <c r="J1798" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1798" s="57">
+        <v>62</v>
+      </c>
+      <c r="L1798" s="88">
+        <v>52.941176470588204</v>
+      </c>
+      <c r="M1798" s="88">
+        <v>69.230769230769198</v>
+      </c>
+      <c r="N1798" s="88">
+        <v>58.3333333333333</v>
+      </c>
+      <c r="O1798" s="88">
+        <v>77.142857142857196</v>
+      </c>
+      <c r="P1798" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1798" s="89">
+        <v>66.6666666666667</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1799" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1799" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1799" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1799" s="55" t="s">
+        <v>1686</v>
+      </c>
+      <c r="E1799" s="55"/>
+      <c r="F1799" s="56">
+        <v>13</v>
+      </c>
+      <c r="G1799" s="56">
+        <v>7</v>
+      </c>
+      <c r="H1799" s="56">
+        <v>12</v>
+      </c>
+      <c r="I1799" s="56">
+        <v>27</v>
+      </c>
+      <c r="J1799" s="56">
+        <v>1</v>
+      </c>
+      <c r="K1799" s="57">
+        <v>60</v>
+      </c>
+      <c r="L1799" s="88">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="M1799" s="88">
+        <v>53.846153846153797</v>
+      </c>
+      <c r="N1799" s="88">
+        <v>50</v>
+      </c>
+      <c r="O1799" s="88">
+        <v>77.142857142857196</v>
+      </c>
+      <c r="P1799" s="88">
+        <v>25</v>
+      </c>
+      <c r="Q1799" s="89">
+        <v>64.516129032258107</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1800" s="54" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1800" s="55" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1800" s="55" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1800" s="55" t="s">
+        <v>1684</v>
+      </c>
+      <c r="E1800" s="55"/>
+      <c r="F1800" s="56">
+        <v>8</v>
+      </c>
+      <c r="G1800" s="56">
+        <v>3</v>
+      </c>
+      <c r="H1800" s="56">
+        <v>7</v>
+      </c>
+      <c r="I1800" s="56">
+        <v>17</v>
+      </c>
+      <c r="J1800" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1800" s="57">
+        <v>38</v>
+      </c>
+      <c r="L1800" s="88">
+        <v>47.058823529411796</v>
+      </c>
+      <c r="M1800" s="88">
+        <v>23.076923076923102</v>
+      </c>
+      <c r="N1800" s="88">
+        <v>29.1666666666667</v>
+      </c>
+      <c r="O1800" s="88">
+        <v>48.571428571428598</v>
+      </c>
+      <c r="P1800" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1800" s="89">
+        <v>40.860215053763397</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1801" s="58" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1801" s="59" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1801" s="59" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D1801" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1801" s="59"/>
+      <c r="F1801" s="60">
+        <v>1</v>
+      </c>
+      <c r="G1801" s="60">
+        <v>2</v>
+      </c>
+      <c r="H1801" s="60">
+        <v>1</v>
+      </c>
+      <c r="I1801" s="60">
+        <v>1</v>
+      </c>
+      <c r="J1801" s="60"/>
+      <c r="K1801" s="61">
+        <v>5</v>
+      </c>
+      <c r="L1801" s="90">
+        <v>5.8823529411764701</v>
+      </c>
+      <c r="M1801" s="90">
+        <v>15.384615384615399</v>
+      </c>
+      <c r="N1801" s="90">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="O1801" s="90">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1801" s="90"/>
+      <c r="Q1801" s="91">
+        <v>5.3763440860215104</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1802" s="26" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1802" s="27" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1802" s="27" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D1802" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1802" s="27" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F1802" s="28">
+        <v>1</v>
+      </c>
+      <c r="G1802" s="28"/>
+      <c r="H1802" s="28"/>
+      <c r="I1802" s="28"/>
+      <c r="J1802" s="28"/>
+      <c r="K1802" s="29">
+        <v>1</v>
+      </c>
+      <c r="L1802" s="74"/>
+      <c r="M1802" s="74"/>
+      <c r="N1802" s="74"/>
+      <c r="O1802" s="74"/>
+      <c r="P1802" s="74"/>
+      <c r="Q1802" s="75"/>
+    </row>
+    <row r="1803" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1803" s="30" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1803" s="31" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1803" s="31" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D1803" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1803" s="31" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F1803" s="32"/>
+      <c r="G1803" s="32"/>
+      <c r="H1803" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1803" s="32"/>
+      <c r="J1803" s="32"/>
+      <c r="K1803" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1803" s="76"/>
+      <c r="M1803" s="76"/>
+      <c r="N1803" s="76"/>
+      <c r="O1803" s="76"/>
+      <c r="P1803" s="76"/>
+      <c r="Q1803" s="77"/>
+    </row>
+    <row r="1804" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1804" s="30" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1804" s="31" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1804" s="31" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D1804" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1804" s="31" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F1804" s="32"/>
+      <c r="G1804" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1804" s="32"/>
+      <c r="I1804" s="32"/>
+      <c r="J1804" s="32"/>
+      <c r="K1804" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1804" s="76"/>
+      <c r="M1804" s="76"/>
+      <c r="N1804" s="76"/>
+      <c r="O1804" s="76"/>
+      <c r="P1804" s="76"/>
+      <c r="Q1804" s="77"/>
+    </row>
+    <row r="1805" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1805" s="30" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1805" s="31" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1805" s="31" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D1805" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1805" s="31" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F1805" s="32"/>
+      <c r="G1805" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1805" s="32"/>
+      <c r="I1805" s="32"/>
+      <c r="J1805" s="32"/>
+      <c r="K1805" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1805" s="76"/>
+      <c r="M1805" s="76"/>
+      <c r="N1805" s="76"/>
+      <c r="O1805" s="76"/>
+      <c r="P1805" s="76"/>
+      <c r="Q1805" s="77"/>
+    </row>
+    <row r="1806" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1806" s="34" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B1806" s="35" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1806" s="35" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D1806" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1806" s="35" t="s">
+        <v>1693</v>
+      </c>
+      <c r="F1806" s="36"/>
+      <c r="G1806" s="36"/>
+      <c r="H1806" s="36"/>
+      <c r="I1806" s="36">
+        <v>1</v>
+      </c>
+      <c r="J1806" s="36"/>
+      <c r="K1806" s="37">
+        <v>1</v>
+      </c>
+      <c r="L1806" s="78"/>
+      <c r="M1806" s="78"/>
+      <c r="N1806" s="78"/>
+      <c r="O1806" s="78"/>
+      <c r="P1806" s="78"/>
+      <c r="Q1806" s="79"/>
+    </row>
+    <row r="1807" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1808" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1808" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1808" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1808" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1808" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1808" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1808" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1808" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1808" s="97" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1808" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1808" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1808" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1808" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1808" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1808" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1808" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1808" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1808" s="99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1809" s="50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1809" s="51" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1809" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1809" s="51" t="s">
+        <v>1697</v>
+      </c>
+      <c r="E1809" s="51"/>
+      <c r="F1809" s="52">
+        <v>13</v>
+      </c>
+      <c r="G1809" s="52">
+        <v>4</v>
+      </c>
+      <c r="H1809" s="52">
+        <v>13</v>
+      </c>
+      <c r="I1809" s="52">
+        <v>16</v>
+      </c>
+      <c r="J1809" s="52">
+        <v>2</v>
+      </c>
+      <c r="K1809" s="53">
+        <v>48</v>
+      </c>
+      <c r="L1809" s="86">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="M1809" s="86">
+        <v>30.769230769230798</v>
+      </c>
+      <c r="N1809" s="86">
+        <v>54.1666666666667</v>
+      </c>
+      <c r="O1809" s="86">
+        <v>45.714285714285701</v>
+      </c>
+      <c r="P1809" s="86">
+        <v>50</v>
+      </c>
+      <c r="Q1809" s="87">
+        <v>51.612903225806399</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1810" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1810" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1810" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1810" s="55" t="s">
+        <v>1698</v>
+      </c>
+      <c r="E1810" s="55"/>
+      <c r="F1810" s="56">
+        <v>11</v>
+      </c>
+      <c r="G1810" s="56">
+        <v>3</v>
+      </c>
+      <c r="H1810" s="56">
+        <v>10</v>
+      </c>
+      <c r="I1810" s="56">
+        <v>17</v>
+      </c>
+      <c r="J1810" s="56"/>
+      <c r="K1810" s="57">
+        <v>41</v>
+      </c>
+      <c r="L1810" s="88">
+        <v>64.705882352941202</v>
+      </c>
+      <c r="M1810" s="88">
+        <v>23.076923076923102</v>
+      </c>
+      <c r="N1810" s="88">
+        <v>41.6666666666667</v>
+      </c>
+      <c r="O1810" s="88">
+        <v>48.571428571428598</v>
+      </c>
+      <c r="P1810" s="88"/>
+      <c r="Q1810" s="89">
+        <v>44.086021505376301</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1811" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1811" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1811" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1811" s="55" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E1811" s="55"/>
+      <c r="F1811" s="56">
+        <v>7</v>
+      </c>
+      <c r="G1811" s="56">
+        <v>3</v>
+      </c>
+      <c r="H1811" s="56">
+        <v>12</v>
+      </c>
+      <c r="I1811" s="56">
+        <v>14</v>
+      </c>
+      <c r="J1811" s="56">
+        <v>2</v>
+      </c>
+      <c r="K1811" s="57">
+        <v>38</v>
+      </c>
+      <c r="L1811" s="88">
+        <v>41.176470588235297</v>
+      </c>
+      <c r="M1811" s="88">
+        <v>23.076923076923102</v>
+      </c>
+      <c r="N1811" s="88">
+        <v>50</v>
+      </c>
+      <c r="O1811" s="88">
+        <v>40</v>
+      </c>
+      <c r="P1811" s="88">
+        <v>50</v>
+      </c>
+      <c r="Q1811" s="89">
+        <v>40.860215053763397</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1812" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1812" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1812" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1812" s="55" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E1812" s="55"/>
+      <c r="F1812" s="56">
+        <v>8</v>
+      </c>
+      <c r="G1812" s="56">
+        <v>4</v>
+      </c>
+      <c r="H1812" s="56">
+        <v>13</v>
+      </c>
+      <c r="I1812" s="56">
+        <v>11</v>
+      </c>
+      <c r="J1812" s="56">
+        <v>1</v>
+      </c>
+      <c r="K1812" s="57">
+        <v>37</v>
+      </c>
+      <c r="L1812" s="88">
+        <v>47.058823529411796</v>
+      </c>
+      <c r="M1812" s="88">
+        <v>30.769230769230798</v>
+      </c>
+      <c r="N1812" s="88">
+        <v>54.1666666666667</v>
+      </c>
+      <c r="O1812" s="88">
+        <v>31.428571428571399</v>
+      </c>
+      <c r="P1812" s="88">
+        <v>25</v>
+      </c>
+      <c r="Q1812" s="89">
+        <v>39.784946236559101</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1813" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1813" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1813" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1813" s="55" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E1813" s="55"/>
+      <c r="F1813" s="56">
+        <v>7</v>
+      </c>
+      <c r="G1813" s="56">
+        <v>3</v>
+      </c>
+      <c r="H1813" s="56">
+        <v>7</v>
+      </c>
+      <c r="I1813" s="56">
+        <v>1</v>
+      </c>
+      <c r="J1813" s="56">
+        <v>1</v>
+      </c>
+      <c r="K1813" s="57">
+        <v>19</v>
+      </c>
+      <c r="L1813" s="88">
+        <v>41.176470588235297</v>
+      </c>
+      <c r="M1813" s="88">
+        <v>23.076923076923102</v>
+      </c>
+      <c r="N1813" s="88">
+        <v>29.1666666666667</v>
+      </c>
+      <c r="O1813" s="88">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1813" s="88">
+        <v>25</v>
+      </c>
+      <c r="Q1813" s="89">
+        <v>20.430107526881699</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1814" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1814" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1814" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1814" s="55" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E1814" s="55"/>
+      <c r="F1814" s="56">
+        <v>6</v>
+      </c>
+      <c r="G1814" s="56">
+        <v>1</v>
+      </c>
+      <c r="H1814" s="56">
+        <v>5</v>
+      </c>
+      <c r="I1814" s="56">
+        <v>1</v>
+      </c>
+      <c r="J1814" s="56"/>
+      <c r="K1814" s="57">
+        <v>13</v>
+      </c>
+      <c r="L1814" s="88">
+        <v>35.294117647058798</v>
+      </c>
+      <c r="M1814" s="88">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1814" s="88">
+        <v>20.8333333333333</v>
+      </c>
+      <c r="O1814" s="88">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1814" s="88"/>
+      <c r="Q1814" s="89">
+        <v>13.9784946236559</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1815" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1815" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1815" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1815" s="55" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1815" s="55"/>
+      <c r="F1815" s="56">
+        <v>3</v>
+      </c>
+      <c r="G1815" s="56">
+        <v>1</v>
+      </c>
+      <c r="H1815" s="56">
+        <v>5</v>
+      </c>
+      <c r="I1815" s="56">
+        <v>1</v>
+      </c>
+      <c r="J1815" s="56"/>
+      <c r="K1815" s="57">
+        <v>10</v>
+      </c>
+      <c r="L1815" s="88">
+        <v>17.647058823529399</v>
+      </c>
+      <c r="M1815" s="88">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1815" s="88">
+        <v>20.8333333333333</v>
+      </c>
+      <c r="O1815" s="88">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1815" s="88"/>
+      <c r="Q1815" s="89">
+        <v>10.752688172042999</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1816" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1816" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1816" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1816" s="55" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E1816" s="55"/>
+      <c r="F1816" s="56">
+        <v>3</v>
+      </c>
+      <c r="G1816" s="56"/>
+      <c r="H1816" s="56">
+        <v>4</v>
+      </c>
+      <c r="I1816" s="56"/>
+      <c r="J1816" s="56"/>
+      <c r="K1816" s="57">
+        <v>7</v>
+      </c>
+      <c r="L1816" s="88">
+        <v>17.647058823529399</v>
+      </c>
+      <c r="M1816" s="88"/>
+      <c r="N1816" s="88">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="O1816" s="88"/>
+      <c r="P1816" s="88"/>
+      <c r="Q1816" s="89">
+        <v>7.5268817204301097</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1817" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1817" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1817" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1817" s="55" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E1817" s="55"/>
+      <c r="F1817" s="56">
+        <v>1</v>
+      </c>
+      <c r="G1817" s="56"/>
+      <c r="H1817" s="56">
+        <v>1</v>
+      </c>
+      <c r="I1817" s="56">
+        <v>1</v>
+      </c>
+      <c r="J1817" s="56"/>
+      <c r="K1817" s="57">
+        <v>3</v>
+      </c>
+      <c r="L1817" s="88">
+        <v>5.8823529411764701</v>
+      </c>
+      <c r="M1817" s="88"/>
+      <c r="N1817" s="88">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="O1817" s="88">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1817" s="88"/>
+      <c r="Q1817" s="89">
+        <v>3.2258064516128999</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1818" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1818" s="55" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1818" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1818" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1818" s="55"/>
+      <c r="F1818" s="56"/>
+      <c r="G1818" s="56">
+        <v>1</v>
+      </c>
+      <c r="H1818" s="56">
+        <v>1</v>
+      </c>
+      <c r="I1818" s="56">
+        <v>3</v>
+      </c>
+      <c r="J1818" s="56">
+        <v>1</v>
+      </c>
+      <c r="K1818" s="57">
+        <v>6</v>
+      </c>
+      <c r="L1818" s="88"/>
+      <c r="M1818" s="88">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1818" s="88">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="O1818" s="88">
+        <v>8.5714285714285694</v>
+      </c>
+      <c r="P1818" s="88">
+        <v>25</v>
+      </c>
+      <c r="Q1818" s="89">
+        <v>6.4516129032258096</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1819" s="58" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1819" s="59" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1819" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1819" s="59" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E1819" s="59"/>
+      <c r="F1819" s="60"/>
+      <c r="G1819" s="60"/>
+      <c r="H1819" s="60"/>
+      <c r="I1819" s="60">
+        <v>1</v>
+      </c>
+      <c r="J1819" s="60"/>
+      <c r="K1819" s="61">
+        <v>1</v>
+      </c>
+      <c r="L1819" s="90"/>
+      <c r="M1819" s="90"/>
+      <c r="N1819" s="90"/>
+      <c r="O1819" s="90">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1819" s="90"/>
+      <c r="Q1819" s="91">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1820" s="26" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1820" s="27" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1820" s="27" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1820" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1820" s="27" t="s">
+        <v>1705</v>
+      </c>
+      <c r="F1820" s="28"/>
+      <c r="G1820" s="28"/>
+      <c r="H1820" s="28"/>
+      <c r="I1820" s="28"/>
+      <c r="J1820" s="28">
+        <v>1</v>
+      </c>
+      <c r="K1820" s="29">
+        <v>1</v>
+      </c>
+      <c r="L1820" s="74"/>
+      <c r="M1820" s="74"/>
+      <c r="N1820" s="74"/>
+      <c r="O1820" s="74"/>
+      <c r="P1820" s="74"/>
+      <c r="Q1820" s="75"/>
+    </row>
+    <row r="1821" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1821" s="30" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1821" s="31" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1821" s="31" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1821" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1821" s="31" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F1821" s="32"/>
+      <c r="G1821" s="32"/>
+      <c r="H1821" s="32"/>
+      <c r="I1821" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1821" s="32"/>
+      <c r="K1821" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1821" s="76"/>
+      <c r="M1821" s="76"/>
+      <c r="N1821" s="76"/>
+      <c r="O1821" s="76"/>
+      <c r="P1821" s="76"/>
+      <c r="Q1821" s="77"/>
+    </row>
+    <row r="1822" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1822" s="30" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1822" s="31" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1822" s="31" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1822" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1822" s="31" t="s">
+        <v>1707</v>
+      </c>
+      <c r="F1822" s="32"/>
+      <c r="G1822" s="32"/>
+      <c r="H1822" s="32"/>
+      <c r="I1822" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1822" s="32"/>
+      <c r="K1822" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1822" s="76"/>
+      <c r="M1822" s="76"/>
+      <c r="N1822" s="76"/>
+      <c r="O1822" s="76"/>
+      <c r="P1822" s="76"/>
+      <c r="Q1822" s="77"/>
+    </row>
+    <row r="1823" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1823" s="30" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1823" s="31" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1823" s="31" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1823" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1823" s="31" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F1823" s="32"/>
+      <c r="G1823" s="32"/>
+      <c r="H1823" s="32"/>
+      <c r="I1823" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1823" s="32"/>
+      <c r="K1823" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1823" s="76"/>
+      <c r="M1823" s="76"/>
+      <c r="N1823" s="76"/>
+      <c r="O1823" s="76"/>
+      <c r="P1823" s="76"/>
+      <c r="Q1823" s="77"/>
+    </row>
+    <row r="1824" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1824" s="30" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1824" s="31" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1824" s="31" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1824" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1824" s="31" t="s">
+        <v>1709</v>
+      </c>
+      <c r="F1824" s="32"/>
+      <c r="G1824" s="32"/>
+      <c r="H1824" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1824" s="32"/>
+      <c r="J1824" s="32"/>
+      <c r="K1824" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1824" s="76"/>
+      <c r="M1824" s="76"/>
+      <c r="N1824" s="76"/>
+      <c r="O1824" s="76"/>
+      <c r="P1824" s="76"/>
+      <c r="Q1824" s="77"/>
+    </row>
+    <row r="1825" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1825" s="34" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1825" s="35" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1825" s="35" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1825" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1825" s="35" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F1825" s="36"/>
+      <c r="G1825" s="36">
+        <v>1</v>
+      </c>
+      <c r="H1825" s="36"/>
+      <c r="I1825" s="36"/>
+      <c r="J1825" s="36"/>
+      <c r="K1825" s="37">
+        <v>1</v>
+      </c>
+      <c r="L1825" s="78"/>
+      <c r="M1825" s="78"/>
+      <c r="N1825" s="78"/>
+      <c r="O1825" s="78"/>
+      <c r="P1825" s="78"/>
+      <c r="Q1825" s="79"/>
+    </row>
+    <row r="1826" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1827" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1827" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1827" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1827" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1827" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1827" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1827" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1827" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1827" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1827" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1827" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1827" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1827" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1827" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1827" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1827" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1827" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1827" s="63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1828" s="26" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1828" s="27" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1828" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1828" s="27"/>
+      <c r="E1828" s="27" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1828" s="28">
+        <v>3</v>
+      </c>
+      <c r="G1828" s="28">
+        <v>2</v>
+      </c>
+      <c r="H1828" s="28">
+        <v>5</v>
+      </c>
+      <c r="I1828" s="28">
+        <v>15</v>
+      </c>
+      <c r="J1828" s="28"/>
+      <c r="K1828" s="29">
+        <v>25</v>
+      </c>
+      <c r="L1828" s="74"/>
+      <c r="M1828" s="74"/>
+      <c r="N1828" s="74"/>
+      <c r="O1828" s="74"/>
+      <c r="P1828" s="74"/>
+      <c r="Q1828" s="75"/>
+    </row>
+    <row r="1829" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1829" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1829" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1829" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1829" s="31"/>
+      <c r="E1829" s="31" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F1829" s="32">
+        <v>2</v>
+      </c>
+      <c r="G1829" s="32"/>
+      <c r="H1829" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1829" s="32"/>
+      <c r="J1829" s="32">
+        <v>1</v>
+      </c>
+      <c r="K1829" s="33">
+        <v>4</v>
+      </c>
+      <c r="L1829" s="76"/>
+      <c r="M1829" s="76"/>
+      <c r="N1829" s="76"/>
+      <c r="O1829" s="76"/>
+      <c r="P1829" s="76"/>
+      <c r="Q1829" s="77"/>
+    </row>
+    <row r="1830" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1830" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1830" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1830" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1830" s="31"/>
+      <c r="E1830" s="31" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F1830" s="32"/>
+      <c r="G1830" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1830" s="32"/>
+      <c r="I1830" s="32">
+        <v>3</v>
+      </c>
+      <c r="J1830" s="32"/>
+      <c r="K1830" s="33">
+        <v>4</v>
+      </c>
+      <c r="L1830" s="76"/>
+      <c r="M1830" s="76"/>
+      <c r="N1830" s="76"/>
+      <c r="O1830" s="76"/>
+      <c r="P1830" s="76"/>
+      <c r="Q1830" s="77"/>
+    </row>
+    <row r="1831" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1831" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1831" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1831" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1831" s="31"/>
+      <c r="E1831" s="31" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1831" s="32">
+        <v>11</v>
+      </c>
+      <c r="G1831" s="32">
+        <v>7</v>
+      </c>
+      <c r="H1831" s="32">
+        <v>7</v>
+      </c>
+      <c r="I1831" s="32">
+        <v>8</v>
+      </c>
+      <c r="J1831" s="32">
+        <v>1</v>
+      </c>
+      <c r="K1831" s="33">
+        <v>34</v>
+      </c>
+      <c r="L1831" s="76"/>
+      <c r="M1831" s="76"/>
+      <c r="N1831" s="76"/>
+      <c r="O1831" s="76"/>
+      <c r="P1831" s="76"/>
+      <c r="Q1831" s="77"/>
+    </row>
+    <row r="1832" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1832" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1832" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1832" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1832" s="31"/>
+      <c r="E1832" s="31" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1832" s="32">
+        <v>1</v>
+      </c>
+      <c r="G1832" s="32"/>
+      <c r="H1832" s="32"/>
+      <c r="I1832" s="32"/>
+      <c r="J1832" s="32"/>
+      <c r="K1832" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1832" s="76"/>
+      <c r="M1832" s="76"/>
+      <c r="N1832" s="76"/>
+      <c r="O1832" s="76"/>
+      <c r="P1832" s="76"/>
+      <c r="Q1832" s="77"/>
+    </row>
+    <row r="1833" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1833" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1833" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1833" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1833" s="31"/>
+      <c r="E1833" s="31" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1833" s="32"/>
+      <c r="G1833" s="32"/>
+      <c r="H1833" s="32"/>
+      <c r="I1833" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1833" s="32"/>
+      <c r="K1833" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1833" s="76"/>
+      <c r="M1833" s="76"/>
+      <c r="N1833" s="76"/>
+      <c r="O1833" s="76"/>
+      <c r="P1833" s="76"/>
+      <c r="Q1833" s="77"/>
+    </row>
+    <row r="1834" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1834" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1834" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1834" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1834" s="31"/>
+      <c r="E1834" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1834" s="32"/>
+      <c r="G1834" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1834" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1834" s="32">
+        <v>2</v>
+      </c>
+      <c r="J1834" s="32"/>
+      <c r="K1834" s="33">
+        <v>4</v>
+      </c>
+      <c r="L1834" s="76"/>
+      <c r="M1834" s="76"/>
+      <c r="N1834" s="76"/>
+      <c r="O1834" s="76"/>
+      <c r="P1834" s="76"/>
+      <c r="Q1834" s="77"/>
+    </row>
+    <row r="1835" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1835" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1835" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1835" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1835" s="31"/>
+      <c r="E1835" s="31" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1835" s="32"/>
+      <c r="G1835" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1835" s="32"/>
+      <c r="I1835" s="32"/>
+      <c r="J1835" s="32"/>
+      <c r="K1835" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1835" s="76"/>
+      <c r="M1835" s="76"/>
+      <c r="N1835" s="76"/>
+      <c r="O1835" s="76"/>
+      <c r="P1835" s="76"/>
+      <c r="Q1835" s="77"/>
+    </row>
+    <row r="1836" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1836" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1836" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1836" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1836" s="31"/>
+      <c r="E1836" s="31" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1836" s="32"/>
+      <c r="G1836" s="32"/>
+      <c r="H1836" s="32"/>
+      <c r="I1836" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1836" s="32"/>
+      <c r="K1836" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1836" s="76"/>
+      <c r="M1836" s="76"/>
+      <c r="N1836" s="76"/>
+      <c r="O1836" s="76"/>
+      <c r="P1836" s="76"/>
+      <c r="Q1836" s="77"/>
+    </row>
+    <row r="1837" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1837" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1837" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1837" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1837" s="31"/>
+      <c r="E1837" s="31" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F1837" s="32"/>
+      <c r="G1837" s="32"/>
+      <c r="H1837" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1837" s="32"/>
+      <c r="J1837" s="32"/>
+      <c r="K1837" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1837" s="76"/>
+      <c r="M1837" s="76"/>
+      <c r="N1837" s="76"/>
+      <c r="O1837" s="76"/>
+      <c r="P1837" s="76"/>
+      <c r="Q1837" s="77"/>
+    </row>
+    <row r="1838" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1838" s="30" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1838" s="31" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1838" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1838" s="31"/>
+      <c r="E1838" s="31" t="s">
+        <v>1722</v>
+      </c>
+      <c r="F1838" s="32"/>
+      <c r="G1838" s="32"/>
+      <c r="H1838" s="32"/>
+      <c r="I1838" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1838" s="32"/>
+      <c r="K1838" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1838" s="76"/>
+      <c r="M1838" s="76"/>
+      <c r="N1838" s="76"/>
+      <c r="O1838" s="76"/>
+      <c r="P1838" s="76"/>
+      <c r="Q1838" s="77"/>
+    </row>
+    <row r="1839" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1839" s="34" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1839" s="35" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1839" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1839" s="35"/>
+      <c r="E1839" s="35" t="s">
+        <v>1723</v>
+      </c>
+      <c r="F1839" s="36"/>
+      <c r="G1839" s="36"/>
+      <c r="H1839" s="36"/>
+      <c r="I1839" s="36">
+        <v>1</v>
+      </c>
+      <c r="J1839" s="36"/>
+      <c r="K1839" s="37">
+        <v>1</v>
+      </c>
+      <c r="L1839" s="78"/>
+      <c r="M1839" s="78"/>
+      <c r="N1839" s="78"/>
+      <c r="O1839" s="78"/>
+      <c r="P1839" s="78"/>
+      <c r="Q1839" s="79"/>
+    </row>
+    <row r="1840" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1841" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1841" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1841" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1841" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1841" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1841" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1841" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1841" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1841" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1841" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1841" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1841" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1841" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1841" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1841" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1841" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1841" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1841" s="63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1842" s="50" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1842" s="51" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1842" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1842" s="51" t="s">
+        <v>1726</v>
+      </c>
+      <c r="E1842" s="51"/>
+      <c r="F1842" s="52">
+        <v>17</v>
+      </c>
+      <c r="G1842" s="52">
+        <v>11</v>
+      </c>
+      <c r="H1842" s="52">
+        <v>22</v>
+      </c>
+      <c r="I1842" s="52">
+        <v>28</v>
+      </c>
+      <c r="J1842" s="52">
+        <v>3</v>
+      </c>
+      <c r="K1842" s="53">
+        <v>81</v>
+      </c>
+      <c r="L1842" s="86">
+        <v>100</v>
+      </c>
+      <c r="M1842" s="86">
+        <v>84.615384615384599</v>
+      </c>
+      <c r="N1842" s="86">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="O1842" s="86">
+        <v>80</v>
+      </c>
+      <c r="P1842" s="86">
+        <v>75</v>
+      </c>
+      <c r="Q1842" s="87">
+        <v>87.096774193548399</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1843" s="54" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1843" s="55" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1843" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1843" s="55" t="s">
+        <v>1727</v>
+      </c>
+      <c r="E1843" s="55"/>
+      <c r="F1843" s="56">
+        <v>12</v>
+      </c>
+      <c r="G1843" s="56">
+        <v>10</v>
+      </c>
+      <c r="H1843" s="56">
+        <v>18</v>
+      </c>
+      <c r="I1843" s="56">
+        <v>33</v>
+      </c>
+      <c r="J1843" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1843" s="57">
+        <v>76</v>
+      </c>
+      <c r="L1843" s="88">
+        <v>70.588235294117695</v>
+      </c>
+      <c r="M1843" s="88">
+        <v>76.923076923076906</v>
+      </c>
+      <c r="N1843" s="88">
+        <v>75</v>
+      </c>
+      <c r="O1843" s="88">
+        <v>94.285714285714306</v>
+      </c>
+      <c r="P1843" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1843" s="89">
+        <v>81.720430107526894</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1844" s="54" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1844" s="55" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1844" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1844" s="55" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E1844" s="55"/>
+      <c r="F1844" s="56">
+        <v>14</v>
+      </c>
+      <c r="G1844" s="56">
+        <v>9</v>
+      </c>
+      <c r="H1844" s="56">
+        <v>18</v>
+      </c>
+      <c r="I1844" s="56">
+        <v>31</v>
+      </c>
+      <c r="J1844" s="56">
+        <v>3</v>
+      </c>
+      <c r="K1844" s="57">
+        <v>75</v>
+      </c>
+      <c r="L1844" s="88">
+        <v>82.352941176470594</v>
+      </c>
+      <c r="M1844" s="88">
+        <v>69.230769230769198</v>
+      </c>
+      <c r="N1844" s="88">
+        <v>75</v>
+      </c>
+      <c r="O1844" s="88">
+        <v>88.571428571428598</v>
+      </c>
+      <c r="P1844" s="88">
+        <v>75</v>
+      </c>
+      <c r="Q1844" s="89">
+        <v>80.645161290322605</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1845" s="54" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1845" s="55" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1845" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1845" s="55" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E1845" s="55"/>
+      <c r="F1845" s="56">
+        <v>6</v>
+      </c>
+      <c r="G1845" s="56">
+        <v>6</v>
+      </c>
+      <c r="H1845" s="56">
+        <v>7</v>
+      </c>
+      <c r="I1845" s="56">
+        <v>16</v>
+      </c>
+      <c r="J1845" s="56">
+        <v>2</v>
+      </c>
+      <c r="K1845" s="57">
+        <v>37</v>
+      </c>
+      <c r="L1845" s="88">
+        <v>35.294117647058798</v>
+      </c>
+      <c r="M1845" s="88">
+        <v>46.153846153846203</v>
+      </c>
+      <c r="N1845" s="88">
+        <v>29.1666666666667</v>
+      </c>
+      <c r="O1845" s="88">
+        <v>45.714285714285701</v>
+      </c>
+      <c r="P1845" s="88">
+        <v>50</v>
+      </c>
+      <c r="Q1845" s="89">
+        <v>39.784946236559101</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1846" s="54" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1846" s="55" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1846" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1846" s="55" t="s">
+        <v>1730</v>
+      </c>
+      <c r="E1846" s="55"/>
+      <c r="F1846" s="56">
+        <v>5</v>
+      </c>
+      <c r="G1846" s="56">
+        <v>1</v>
+      </c>
+      <c r="H1846" s="56">
+        <v>7</v>
+      </c>
+      <c r="I1846" s="56">
+        <v>20</v>
+      </c>
+      <c r="J1846" s="56">
+        <v>2</v>
+      </c>
+      <c r="K1846" s="57">
+        <v>35</v>
+      </c>
+      <c r="L1846" s="88">
+        <v>29.411764705882401</v>
+      </c>
+      <c r="M1846" s="88">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1846" s="88">
+        <v>29.1666666666667</v>
+      </c>
+      <c r="O1846" s="88">
+        <v>57.142857142857103</v>
+      </c>
+      <c r="P1846" s="88">
+        <v>50</v>
+      </c>
+      <c r="Q1846" s="89">
+        <v>37.634408602150501</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1847" s="54" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1847" s="55" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1847" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1847" s="55" t="s">
+        <v>1731</v>
+      </c>
+      <c r="E1847" s="55"/>
+      <c r="F1847" s="56">
+        <v>2</v>
+      </c>
+      <c r="G1847" s="56">
+        <v>1</v>
+      </c>
+      <c r="H1847" s="56">
+        <v>3</v>
+      </c>
+      <c r="I1847" s="56"/>
+      <c r="J1847" s="56"/>
+      <c r="K1847" s="57">
+        <v>6</v>
+      </c>
+      <c r="L1847" s="88">
+        <v>11.764705882352899</v>
+      </c>
+      <c r="M1847" s="88">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1847" s="88">
+        <v>12.5</v>
+      </c>
+      <c r="O1847" s="88"/>
+      <c r="P1847" s="88"/>
+      <c r="Q1847" s="89">
+        <v>6.4516129032258096</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1848" s="58" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1848" s="59" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1848" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1848" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1848" s="59"/>
+      <c r="F1848" s="60"/>
+      <c r="G1848" s="60">
+        <v>3</v>
+      </c>
+      <c r="H1848" s="60">
+        <v>3</v>
+      </c>
+      <c r="I1848" s="60">
+        <v>6</v>
+      </c>
+      <c r="J1848" s="60"/>
+      <c r="K1848" s="61">
+        <v>12</v>
+      </c>
+      <c r="L1848" s="90"/>
+      <c r="M1848" s="90">
+        <v>23.076923076923102</v>
+      </c>
+      <c r="N1848" s="90">
+        <v>12.5</v>
+      </c>
+      <c r="O1848" s="90">
+        <v>17.1428571428571</v>
+      </c>
+      <c r="P1848" s="90"/>
+      <c r="Q1848" s="91">
+        <v>12.9032258064516</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1849" s="26" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1849" s="27" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1849" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1849" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1849" s="27" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F1849" s="28"/>
+      <c r="G1849" s="28"/>
+      <c r="H1849" s="28"/>
+      <c r="I1849" s="28">
+        <v>1</v>
+      </c>
+      <c r="J1849" s="28"/>
+      <c r="K1849" s="29">
+        <v>1</v>
+      </c>
+      <c r="L1849" s="74"/>
+      <c r="M1849" s="74"/>
+      <c r="N1849" s="74"/>
+      <c r="O1849" s="74"/>
+      <c r="P1849" s="74"/>
+      <c r="Q1849" s="75"/>
+    </row>
+    <row r="1850" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1850" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1850" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1850" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1850" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1850" s="31" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F1850" s="32"/>
+      <c r="G1850" s="32"/>
+      <c r="H1850" s="32"/>
+      <c r="I1850" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1850" s="32"/>
+      <c r="K1850" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1850" s="76"/>
+      <c r="M1850" s="76"/>
+      <c r="N1850" s="76"/>
+      <c r="O1850" s="76"/>
+      <c r="P1850" s="76"/>
+      <c r="Q1850" s="77"/>
+    </row>
+    <row r="1851" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1851" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1851" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1851" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1851" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1851" s="31" t="s">
+        <v>1734</v>
+      </c>
+      <c r="F1851" s="32"/>
+      <c r="G1851" s="32"/>
+      <c r="H1851" s="32"/>
+      <c r="I1851" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1851" s="32"/>
+      <c r="K1851" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1851" s="76"/>
+      <c r="M1851" s="76"/>
+      <c r="N1851" s="76"/>
+      <c r="O1851" s="76"/>
+      <c r="P1851" s="76"/>
+      <c r="Q1851" s="77"/>
+    </row>
+    <row r="1852" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1852" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1852" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1852" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1852" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1852" s="31" t="s">
+        <v>1735</v>
+      </c>
+      <c r="F1852" s="32"/>
+      <c r="G1852" s="32"/>
+      <c r="H1852" s="32"/>
+      <c r="I1852" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1852" s="32"/>
+      <c r="K1852" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1852" s="76"/>
+      <c r="M1852" s="76"/>
+      <c r="N1852" s="76"/>
+      <c r="O1852" s="76"/>
+      <c r="P1852" s="76"/>
+      <c r="Q1852" s="77"/>
+    </row>
+    <row r="1853" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1853" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1853" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1853" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1853" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1853" s="31" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F1853" s="32"/>
+      <c r="G1853" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1853" s="32"/>
+      <c r="I1853" s="32"/>
+      <c r="J1853" s="32"/>
+      <c r="K1853" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1853" s="76"/>
+      <c r="M1853" s="76"/>
+      <c r="N1853" s="76"/>
+      <c r="O1853" s="76"/>
+      <c r="P1853" s="76"/>
+      <c r="Q1853" s="77"/>
+    </row>
+    <row r="1854" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1854" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1854" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1854" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1854" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1854" s="31" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F1854" s="32"/>
+      <c r="G1854" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1854" s="32"/>
+      <c r="I1854" s="32"/>
+      <c r="J1854" s="32"/>
+      <c r="K1854" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1854" s="76"/>
+      <c r="M1854" s="76"/>
+      <c r="N1854" s="76"/>
+      <c r="O1854" s="76"/>
+      <c r="P1854" s="76"/>
+      <c r="Q1854" s="77"/>
+    </row>
+    <row r="1855" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1855" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1855" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1855" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1855" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1855" s="31" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F1855" s="32"/>
+      <c r="G1855" s="32"/>
+      <c r="H1855" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1855" s="32"/>
+      <c r="J1855" s="32"/>
+      <c r="K1855" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1855" s="76"/>
+      <c r="M1855" s="76"/>
+      <c r="N1855" s="76"/>
+      <c r="O1855" s="76"/>
+      <c r="P1855" s="76"/>
+      <c r="Q1855" s="77"/>
+    </row>
+    <row r="1856" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1856" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1856" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1856" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1856" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1856" s="31" t="s">
+        <v>1739</v>
+      </c>
+      <c r="F1856" s="32"/>
+      <c r="G1856" s="32"/>
+      <c r="H1856" s="32">
+        <v>1</v>
+      </c>
+      <c r="I1856" s="32"/>
+      <c r="J1856" s="32"/>
+      <c r="K1856" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1856" s="76"/>
+      <c r="M1856" s="76"/>
+      <c r="N1856" s="76"/>
+      <c r="O1856" s="76"/>
+      <c r="P1856" s="76"/>
+      <c r="Q1856" s="77"/>
+    </row>
+    <row r="1857" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1857" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1857" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1857" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1857" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1857" s="31" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F1857" s="32"/>
+      <c r="G1857" s="32">
+        <v>1</v>
+      </c>
+      <c r="H1857" s="32"/>
+      <c r="I1857" s="32"/>
+      <c r="J1857" s="32"/>
+      <c r="K1857" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1857" s="76"/>
+      <c r="M1857" s="76"/>
+      <c r="N1857" s="76"/>
+      <c r="O1857" s="76"/>
+      <c r="P1857" s="76"/>
+      <c r="Q1857" s="77"/>
+    </row>
+    <row r="1858" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1858" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1858" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1858" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1858" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1858" s="31" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F1858" s="32"/>
+      <c r="G1858" s="32"/>
+      <c r="H1858" s="32"/>
+      <c r="I1858" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1858" s="32"/>
+      <c r="K1858" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1858" s="76"/>
+      <c r="M1858" s="76"/>
+      <c r="N1858" s="76"/>
+      <c r="O1858" s="76"/>
+      <c r="P1858" s="76"/>
+      <c r="Q1858" s="77"/>
+    </row>
+    <row r="1859" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1859" s="30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1859" s="31" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1859" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1859" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1859" s="31" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F1859" s="32"/>
+      <c r="G1859" s="32"/>
+      <c r="H1859" s="32"/>
+      <c r="I1859" s="32">
+        <v>1</v>
+      </c>
+      <c r="J1859" s="32"/>
+      <c r="K1859" s="33">
+        <v>1</v>
+      </c>
+      <c r="L1859" s="76"/>
+      <c r="M1859" s="76"/>
+      <c r="N1859" s="76"/>
+      <c r="O1859" s="76"/>
+      <c r="P1859" s="76"/>
+      <c r="Q1859" s="77"/>
+    </row>
+    <row r="1860" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1860" s="34" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B1860" s="35" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1860" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1860" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1860" s="35" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F1860" s="36"/>
+      <c r="G1860" s="36"/>
+      <c r="H1860" s="36">
+        <v>1</v>
+      </c>
+      <c r="I1860" s="36"/>
+      <c r="J1860" s="36"/>
+      <c r="K1860" s="37">
+        <v>1</v>
+      </c>
+      <c r="L1860" s="78"/>
+      <c r="M1860" s="78"/>
+      <c r="N1860" s="78"/>
+      <c r="O1860" s="78"/>
+      <c r="P1860" s="78"/>
+      <c r="Q1860" s="79"/>
+    </row>
+    <row r="1862" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1862" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1862" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1862" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1862" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1862" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1862" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1862" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1862" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1862" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1862" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1862" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1862" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1862" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1862" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1862" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1862" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1862" s="71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1863" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1863" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1863" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1863" s="1" t="s">
+        <v>1746</v>
+      </c>
+      <c r="J1863" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1863" s="21">
+        <v>1</v>
+      </c>
+      <c r="P1863" s="70">
+        <v>25</v>
+      </c>
+      <c r="Q1863" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1864" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1864" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1864" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1864" s="1" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F1864" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1864" s="2">
+        <v>3</v>
+      </c>
+      <c r="I1864" s="2">
+        <v>3</v>
+      </c>
+      <c r="J1864" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1864" s="21">
+        <v>9</v>
+      </c>
+      <c r="L1864" s="70">
+        <v>11.764705882352899</v>
+      </c>
+      <c r="N1864" s="70">
+        <v>12.5</v>
+      </c>
+      <c r="O1864" s="70">
+        <v>8.5714285714285694</v>
+      </c>
+      <c r="P1864" s="70">
+        <v>25</v>
+      </c>
+      <c r="Q1864" s="71">
+        <v>9.67741935483871</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1865" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1865" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1865" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1865" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="G1865" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1865" s="21">
+        <v>1</v>
+      </c>
+      <c r="M1865" s="70">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="Q1865" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1866" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1866" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1866" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1866" s="1" t="s">
+        <v>1749</v>
+      </c>
+      <c r="I1866" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1866" s="21">
+        <v>1</v>
+      </c>
+      <c r="O1866" s="70">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="Q1866" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1867" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1867" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1867" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1867" s="1" t="s">
+        <v>1750</v>
+      </c>
+      <c r="J1867" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1867" s="21">
+        <v>1</v>
+      </c>
+      <c r="P1867" s="70">
+        <v>25</v>
+      </c>
+      <c r="Q1867" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1868" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1868" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1868" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1868" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="G1868" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1868" s="21">
+        <v>1</v>
+      </c>
+      <c r="M1868" s="70">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="Q1868" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1869" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1869" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1869" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1869" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="I1869" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1869" s="21">
+        <v>1</v>
+      </c>
+      <c r="O1869" s="70">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="Q1869" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1870" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1870" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1870" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1870" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="G1870" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1870" s="21">
+        <v>1</v>
+      </c>
+      <c r="M1870" s="70">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="Q1870" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1871" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1871" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1871" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1871" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="G1871" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1871" s="21">
+        <v>1</v>
+      </c>
+      <c r="M1871" s="70">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="Q1871" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1872" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1872" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1872" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1872" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="H1872" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1872" s="21">
+        <v>1</v>
+      </c>
+      <c r="N1872" s="70">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="Q1872" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1873" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1873" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1873" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1873" s="1" t="s">
+        <v>1756</v>
+      </c>
+      <c r="G1873" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1873" s="2">
+        <v>3</v>
+      </c>
+      <c r="I1873" s="2">
+        <v>6</v>
+      </c>
+      <c r="K1873" s="21">
+        <v>11</v>
+      </c>
+      <c r="M1873" s="70">
+        <v>15.384615384615399</v>
+      </c>
+      <c r="N1873" s="70">
+        <v>12.5</v>
+      </c>
+      <c r="O1873" s="70">
+        <v>17.1428571428571</v>
+      </c>
+      <c r="Q1873" s="71">
+        <v>11.8279569892473</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1874" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1874" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1874" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1874" s="1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="F1874" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1874" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1874" s="2">
+        <v>1</v>
+      </c>
+      <c r="I1874" s="2">
+        <v>5</v>
+      </c>
+      <c r="K1874" s="21">
+        <v>11</v>
+      </c>
+      <c r="L1874" s="70">
+        <v>23.529411764705898</v>
+      </c>
+      <c r="M1874" s="70">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1874" s="70">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="O1874" s="70">
+        <v>14.285714285714301</v>
+      </c>
+      <c r="Q1874" s="71">
+        <v>11.8279569892473</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1875" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1875" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1875" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1875" s="1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="F1875" s="2">
+        <v>11</v>
+      </c>
+      <c r="G1875" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1875" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1875" s="2">
+        <v>1</v>
+      </c>
+      <c r="J1875" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1875" s="21">
+        <v>22</v>
+      </c>
+      <c r="L1875" s="70">
+        <v>64.705882352941202</v>
+      </c>
+      <c r="M1875" s="70">
+        <v>15.384615384615399</v>
+      </c>
+      <c r="N1875" s="70">
+        <v>29.1666666666667</v>
+      </c>
+      <c r="O1875" s="70">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="P1875" s="70">
+        <v>25</v>
+      </c>
+      <c r="Q1875" s="71">
+        <v>23.655913978494599</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1876" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1876" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1876" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1876" s="1" t="s">
+        <v>1759</v>
+      </c>
+      <c r="I1876" s="2">
+        <v>2</v>
+      </c>
+      <c r="K1876" s="21">
+        <v>2</v>
+      </c>
+      <c r="O1876" s="70">
+        <v>5.71428571428571</v>
+      </c>
+      <c r="Q1876" s="71">
+        <v>2.1505376344085998</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1877" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1877" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1877" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1877" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="G1877" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1877" s="2">
+        <v>1</v>
+      </c>
+      <c r="I1877" s="2">
+        <v>3</v>
+      </c>
+      <c r="K1877" s="21">
+        <v>5</v>
+      </c>
+      <c r="M1877" s="70">
+        <v>7.6923076923076898</v>
+      </c>
+      <c r="N1877" s="70">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="O1877" s="70">
+        <v>8.5714285714285694</v>
+      </c>
+      <c r="Q1877" s="71">
+        <v>5.3763440860215104</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1878" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1878" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1878" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1878" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="H1878" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1878" s="21">
+        <v>1</v>
+      </c>
+      <c r="N1878" s="70">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="Q1878" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1879" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1879" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1879" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1879" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="G1879" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1879" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1879" s="2">
+        <v>11</v>
+      </c>
+      <c r="K1879" s="21">
+        <v>20</v>
+      </c>
+      <c r="M1879" s="70">
+        <v>23.076923076923102</v>
+      </c>
+      <c r="N1879" s="70">
+        <v>25</v>
+      </c>
+      <c r="O1879" s="70">
+        <v>31.428571428571399</v>
+      </c>
+      <c r="Q1879" s="71">
+        <v>21.505376344085999</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1880" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1880" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1880" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1880" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="H1880" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1880" s="21">
+        <v>1</v>
+      </c>
+      <c r="N1880" s="70">
+        <v>4.1666666666666696</v>
+      </c>
+      <c r="Q1880" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1881" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1881" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1881" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1881" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="I1881" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1881" s="21">
+        <v>1</v>
+      </c>
+      <c r="O1881" s="70">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="Q1881" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1882" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B1882" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1882" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1882" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="I1882" s="2">
+        <v>1</v>
+      </c>
+      <c r="K1882" s="21">
+        <v>1</v>
+      </c>
+      <c r="O1882" s="70">
+        <v>2.8571428571428599</v>
+      </c>
+      <c r="Q1882" s="71">
+        <v>1.0752688172042999</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1676:Q1682">
-    <sortCondition descending="1" ref="Q1676"/>
+  <sortState ref="A1842:Q1847">
+    <sortCondition descending="1" ref="Q1842"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>